<commit_message>
added distance sensor calibration
</commit_message>
<xml_diff>
--- a/Documents/Distance sensor measurements.xlsx
+++ b/Documents/Distance sensor measurements.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\badboy\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\NXP-CUP\NXP-Cup\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664E5FC4-B02F-4E97-8F17-F9BEBE77FBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E20FB8-3B05-40E4-BBC9-3C0248550464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Vcc</t>
   </si>
@@ -55,10 +56,34 @@
     <t>Measured cm</t>
   </si>
   <si>
-    <t>distance from sensor to front of the car [cm]</t>
+    <t>generated</t>
   </si>
   <si>
-    <t>generated</t>
+    <t>c</t>
+  </si>
+  <si>
+    <t>offset</t>
+  </si>
+  <si>
+    <t>sensor_data*x</t>
+  </si>
+  <si>
+    <t>calibrated_data = sensor_data - offset</t>
+  </si>
+  <si>
+    <t>offset =</t>
+  </si>
+  <si>
+    <t>Real [m]</t>
+  </si>
+  <si>
+    <t>Measured [m]</t>
+  </si>
+  <si>
+    <t>calibrated data [m]</t>
+  </si>
+  <si>
+    <t>distance from sensor to front of the car [m]</t>
   </si>
 </sst>
 </file>
@@ -128,6 +153,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>data</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -172,7 +222,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Real cm</c:v>
+                  <c:v>Real [m]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -203,63 +253,54 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$19</c:f>
+              <c:f>Sheet2!$A$2:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14</c:v>
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>60</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>70</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>80</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>90</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>100</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>110</c:v>
+                  <c:v>1.1000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>150</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -280,7 +321,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Measured cm</c:v>
+                  <c:v>Measured [m]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -311,63 +352,54 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$19</c:f>
+              <c:f>Sheet2!$B$2:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>1.2</c:v>
+                  <c:v>1.2E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.6</c:v>
+                  <c:v>0.126</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19.8</c:v>
+                  <c:v>0.19800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.8</c:v>
+                  <c:v>0.28800000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36</c:v>
+                  <c:v>0.36</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>49.2</c:v>
+                  <c:v>0.49200000000000005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>59.4</c:v>
+                  <c:v>0.59399999999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>66.599999999999994</c:v>
+                  <c:v>0.66599999999999993</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>75.599999999999994</c:v>
+                  <c:v>0.75599999999999989</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>84.6</c:v>
+                  <c:v>0.84599999999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>93.6</c:v>
+                  <c:v>0.93599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>102.6</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>111.6</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>120.6</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>127.2</c:v>
+                  <c:v>1.272</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -376,6 +408,105 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8B4A-4E1D-AA45-47AC909BD4EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>calibrated data [m]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$2:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>6.9488000000000008E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11220000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15715999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16839999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.19762400000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.27855200000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.37971200000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.46063999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.60900799999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.72365599999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.80458399999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.90574399999999988</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.006904</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1080639999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4857279999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-882B-4F13-977E-0AE8EE563E2E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1128,16 +1259,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>11430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>11430</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1487,10 +1618,313 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A28E291-0E5A-42FB-A48A-EF8E534ECA3D}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" customWidth="1"/>
+    <col min="5" max="5" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B2">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C2">
+        <f>B2-(B2*$H$3 + $I$3)</f>
+        <v>6.9488000000000008E-2</v>
+      </c>
+      <c r="D2">
+        <f>C2-A2</f>
+        <v>-5.1199999999999857E-4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0.1</v>
+      </c>
+      <c r="B3">
+        <v>0.05</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C16" si="0">B3-(B3*$H$3 + $I$3)</f>
+        <v>0.11220000000000001</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D16" si="1">C3-A3</f>
+        <v>1.2200000000000003E-2</v>
+      </c>
+      <c r="E3">
+        <v>0.06</v>
+      </c>
+      <c r="H3">
+        <v>-0.124</v>
+      </c>
+      <c r="I3">
+        <v>-5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="B4">
+        <v>0.09</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0.15715999999999999</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>1.7159999999999981E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0.16</v>
+      </c>
+      <c r="B5">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.16839999999999999</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>8.3999999999999908E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0.2</v>
+      </c>
+      <c r="B6">
+        <v>0.126</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.19762400000000002</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>-2.3759999999999892E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0.3</v>
+      </c>
+      <c r="B7">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0.27855200000000002</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>-2.1447999999999967E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0.4</v>
+      </c>
+      <c r="B8">
+        <v>0.28800000000000003</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0.37971200000000005</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>-2.0287999999999973E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0.5</v>
+      </c>
+      <c r="B9">
+        <v>0.36</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.46063999999999999</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>-3.9360000000000006E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0.6</v>
+      </c>
+      <c r="B10">
+        <v>0.49200000000000005</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0.60900799999999999</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>9.008000000000016E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0.7</v>
+      </c>
+      <c r="B11">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0.72365599999999997</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>2.365600000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0.8</v>
+      </c>
+      <c r="B12">
+        <v>0.66599999999999993</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0.80458399999999997</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>4.5839999999999215E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0.9</v>
+      </c>
+      <c r="B13">
+        <v>0.75599999999999989</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0.90574399999999988</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>5.7439999999998603E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>1.006904</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>6.9040000000000212E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B15">
+        <v>0.93599999999999994</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>1.1080639999999999</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>8.0639999999998491E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1.5</v>
+      </c>
+      <c r="B16">
+        <v>1.272</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>1.4857279999999999</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>-1.4272000000000062E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAED98AF-3C09-4107-BEE4-7B0781F7D458}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1500,7 +1934,7 @@
     <col min="5" max="5" width="38.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1508,125 +1942,175 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>7</v>
       </c>
       <c r="B2">
         <v>1.2</v>
       </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <f>B2/100</f>
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <f t="shared" ref="D3:D19" si="0">B3/100</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>14</v>
       </c>
       <c r="B4">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>16</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>20</v>
       </c>
       <c r="B6">
         <v>12.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>30</v>
       </c>
       <c r="B7">
         <v>19.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.19800000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>40</v>
       </c>
       <c r="B8">
         <v>28.8</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.28800000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>50</v>
       </c>
       <c r="B9">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>60</v>
       </c>
       <c r="B10">
         <v>49.2</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0.49200000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>70</v>
       </c>
       <c r="B11">
         <v>59.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0.59399999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>80</v>
       </c>
       <c r="B12">
         <v>66.599999999999994</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0.66599999999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>90</v>
       </c>
       <c r="B13">
         <v>75.599999999999994</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0.75599999999999989</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>100</v>
       </c>
       <c r="B14">
         <v>84.6</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0.84599999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>110</v>
       </c>
       <c r="B15">
         <v>93.6</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0.93599999999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>120</v>
       </c>
@@ -1634,10 +2118,14 @@
         <v>102.6</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>1.026</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>130</v>
       </c>
@@ -1645,10 +2133,14 @@
         <v>111.6</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>1.1159999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>140</v>
       </c>
@@ -1656,19 +2148,27 @@
         <v>120.6</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>1.206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>150</v>
       </c>
       <c r="B19">
         <v>127.2</v>
       </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>1.272</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>